<commit_message>
Upload and download file done
</commit_message>
<xml_diff>
--- a/Back-end/sheetmanager/file_example_XLSX_100.xlsx_2.xlsx
+++ b/Back-end/sheetmanager/file_example_XLSX_100.xlsx_2.xlsx
@@ -12,28 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>Teresa</t>
   </si>
@@ -171,6 +150,12 @@
   </si>
   <si>
     <t>Pfau</t>
+  </si>
+  <si>
+    <t>Shanice</t>
+  </si>
+  <si>
+    <t>Mccrystal</t>
   </si>
 </sst>
 </file>
@@ -223,7 +208,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n" s="0">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="B1" t="s" s="0">
         <v>0</v>
@@ -237,115 +222,115 @@
       <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="0">
-        <v>4</v>
+      <c r="F1" t="n" s="0">
+        <v>46.0</v>
       </c>
       <c r="G1" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="H1" t="n" s="0">
+        <v>3569.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="B2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="F2" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="G2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>46.0</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>11</v>
-      </c>
       <c r="H2" t="n" s="0">
-        <v>3569.0</v>
+        <v>2564.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>37.0</v>
+        <v>52.0</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>2564.0</v>
+        <v>8561.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>14</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>52.0</v>
+        <v>46.0</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>8561.0</v>
+        <v>5489.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>46.0</v>
+        <v>42.0</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H5" t="n" s="0">
         <v>5489.0</v>
@@ -353,392 +338,392 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>42.0</v>
+        <v>21.0</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>5489.0</v>
+        <v>6574.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>21.0</v>
+        <v>28.0</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H7" t="n" s="0">
-        <v>6574.0</v>
+        <v>5555.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n" s="0">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>5555.0</v>
+        <v>6125.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n" s="0">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>29.0</v>
+        <v>23.0</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>6125.0</v>
+        <v>5412.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n" s="0">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>23.0</v>
+        <v>41.0</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>5412.0</v>
+        <v>3256.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n" s="0">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s" s="0">
         <v>14</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>41.0</v>
+        <v>28.0</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>3256.0</v>
+        <v>3264.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n" s="0">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>28.0</v>
+        <v>37.0</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H12" t="n" s="0">
-        <v>3264.0</v>
+        <v>4569.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n" s="0">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>37.0</v>
+        <v>34.0</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H13" t="n" s="0">
-        <v>4569.0</v>
+        <v>7521.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n" s="0">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>34.0</v>
+        <v>26.0</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H14" t="n" s="0">
-        <v>7521.0</v>
+        <v>6458.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n" s="0">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>26.0</v>
+        <v>35.0</v>
       </c>
       <c r="G15" t="s" s="0">
         <v>11</v>
       </c>
       <c r="H15" t="n" s="0">
-        <v>6458.0</v>
+        <v>7569.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n" s="0">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H16" t="n" s="0">
-        <v>7569.0</v>
+        <v>8514.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n" s="0">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>36.0</v>
+        <v>29.0</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H17" t="n" s="0">
-        <v>8514.0</v>
+        <v>8563.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n" s="0">
-        <v>36.0</v>
+        <v>37.0</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n" s="0">
-        <v>29.0</v>
+        <v>27.0</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H18" t="n" s="0">
-        <v>8563.0</v>
+        <v>8642.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n" s="0">
-        <v>37.0</v>
+        <v>38.0</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n" s="0">
-        <v>27.0</v>
+        <v>25.0</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="H19" t="n" s="0">
-        <v>8642.0</v>
+        <v>9536.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n" s="0">
-        <v>38.0</v>
+        <v>39.0</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n" s="0">
-        <v>25.0</v>
+        <v>36.0</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H20" t="n" s="0">
-        <v>9536.0</v>
+        <v>2567.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>